<commit_message>
modified:   Brighway/Monte_Carlo.py 	new file:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_CDU.jpg 	new file:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_MDU.jpg 	new file:   Brighway/Single-use-vs-multi-use-in-health-care/Results/MC_results_No DU.jpg 	new file:   Brighway/__pycache__/LCA.cpython-311.pyc 	modified:   Brighway/__pycache__/Monte_Carlo.cpython-311.pyc 	new file:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/climate change -monte_carlo_simulations_Rune.xlsx 	new file:   Brighway/life_cycle_assessment.py
</commit_message>
<xml_diff>
--- a/Brighway/climate change -monte_carlo_simulations_Rune.xlsx
+++ b/Brighway/climate change -monte_carlo_simulations_Rune.xlsx
@@ -417,13 +417,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>707.1534062399148</v>
+        <v>653.9476226199286</v>
       </c>
       <c r="C2">
-        <v>116.0226722034306</v>
+        <v>136.3288556572895</v>
       </c>
       <c r="D2">
-        <v>102.2714299913569</v>
+        <v>85.96170863986495</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -431,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>707.1534062399148</v>
+        <v>653.9476226199286</v>
       </c>
       <c r="C3">
-        <v>116.0226722034306</v>
+        <v>136.3288556572895</v>
       </c>
       <c r="D3">
-        <v>102.2714299913569</v>
+        <v>85.96170863986495</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -445,13 +445,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>52.28612303773298</v>
+        <v>28.80387728896227</v>
       </c>
       <c r="C4">
-        <v>35.47747379154359</v>
+        <v>46.71042583927353</v>
       </c>
       <c r="D4">
-        <v>13.6187720798948</v>
+        <v>0.826043741803197</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -459,13 +459,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>654.8672832021819</v>
+        <v>625.1437453309662</v>
       </c>
       <c r="C5">
-        <v>80.54519841188703</v>
+        <v>89.61842981801597</v>
       </c>
       <c r="D5">
-        <v>88.65265791146206</v>
+        <v>85.13566489806176</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -473,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>759.4395292776478</v>
+        <v>682.7514999088908</v>
       </c>
       <c r="C6">
-        <v>151.5001459949742</v>
+        <v>183.039281496563</v>
       </c>
       <c r="D6">
-        <v>115.8902020712517</v>
+        <v>86.78775238166816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>